<commit_message>
feat: include ghg breakdown in ecrf generated file
</commit_message>
<xml_diff>
--- a/app/templates/ecrf_template.xlsx
+++ b/app/templates/ecrf_template.xlsx
@@ -685,12 +685,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -718,13 +724,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -744,37 +750,37 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="4" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -794,6 +800,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffa5a5a5"/>
     </indexedColors>
   </colors>
@@ -7841,39 +7848,19 @@
       <c r="E66" t="s" s="3">
         <v>134</v>
       </c>
-      <c r="F66" t="s" s="3">
-        <v>116</v>
-      </c>
+      <c r="F66" s="3"/>
       <c r="G66" t="s" s="3">
-        <v>117</v>
-      </c>
-      <c r="H66" t="s" s="3">
-        <v>118</v>
-      </c>
-      <c r="I66" t="s" s="3">
-        <v>119</v>
-      </c>
-      <c r="J66" t="s" s="3">
-        <v>120</v>
-      </c>
-      <c r="K66" t="s" s="3">
-        <v>121</v>
-      </c>
-      <c r="L66" t="s" s="3">
-        <v>122</v>
-      </c>
-      <c r="M66" t="s" s="3">
-        <v>123</v>
-      </c>
-      <c r="N66" t="s" s="3">
-        <v>124</v>
-      </c>
-      <c r="O66" t="s" s="3">
-        <v>125</v>
-      </c>
-      <c r="P66" t="s" s="3">
-        <v>126</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+      <c r="P66" s="3"/>
       <c r="Q66" s="2"/>
       <c r="R66" s="2"/>
       <c r="S66" s="2"/>
@@ -7882,18 +7869,10 @@
       <c r="V66" s="2"/>
       <c r="W66" s="2"/>
       <c r="X66" s="2"/>
-      <c r="Y66" t="s" s="3">
-        <v>127</v>
-      </c>
-      <c r="Z66" t="s" s="3">
-        <v>128</v>
-      </c>
-      <c r="AA66" t="s" s="3">
-        <v>129</v>
-      </c>
-      <c r="AB66" t="s" s="3">
-        <v>130</v>
-      </c>
+      <c r="Y66" s="3"/>
+      <c r="Z66" s="3"/>
+      <c r="AA66" s="3"/>
+      <c r="AB66" s="3"/>
       <c r="AC66" s="2"/>
       <c r="AD66" s="12"/>
       <c r="AE66" s="12"/>
@@ -7914,39 +7893,19 @@
       <c r="E67" t="s" s="3">
         <v>134</v>
       </c>
-      <c r="F67" t="s" s="3">
-        <v>116</v>
-      </c>
+      <c r="F67" s="3"/>
       <c r="G67" t="s" s="3">
-        <v>117</v>
-      </c>
-      <c r="H67" t="s" s="3">
-        <v>118</v>
-      </c>
-      <c r="I67" t="s" s="3">
-        <v>119</v>
-      </c>
-      <c r="J67" t="s" s="3">
-        <v>120</v>
-      </c>
-      <c r="K67" t="s" s="3">
-        <v>121</v>
-      </c>
-      <c r="L67" t="s" s="3">
-        <v>122</v>
-      </c>
-      <c r="M67" t="s" s="3">
-        <v>123</v>
-      </c>
-      <c r="N67" t="s" s="3">
-        <v>124</v>
-      </c>
-      <c r="O67" t="s" s="3">
-        <v>125</v>
-      </c>
-      <c r="P67" t="s" s="3">
-        <v>126</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
       <c r="S67" s="2"/>
@@ -7955,18 +7914,10 @@
       <c r="V67" s="2"/>
       <c r="W67" s="2"/>
       <c r="X67" s="2"/>
-      <c r="Y67" t="s" s="3">
-        <v>127</v>
-      </c>
-      <c r="Z67" t="s" s="3">
-        <v>128</v>
-      </c>
-      <c r="AA67" t="s" s="3">
-        <v>129</v>
-      </c>
-      <c r="AB67" t="s" s="3">
-        <v>130</v>
-      </c>
+      <c r="Y67" s="3"/>
+      <c r="Z67" s="3"/>
+      <c r="AA67" s="3"/>
+      <c r="AB67" s="3"/>
       <c r="AC67" s="2"/>
       <c r="AD67" s="12"/>
       <c r="AE67" s="12"/>
@@ -7987,39 +7938,19 @@
       <c r="E68" t="s" s="3">
         <v>134</v>
       </c>
-      <c r="F68" t="s" s="3">
-        <v>116</v>
-      </c>
+      <c r="F68" s="3"/>
       <c r="G68" t="s" s="3">
-        <v>117</v>
-      </c>
-      <c r="H68" t="s" s="3">
-        <v>118</v>
-      </c>
-      <c r="I68" t="s" s="3">
-        <v>119</v>
-      </c>
-      <c r="J68" t="s" s="3">
-        <v>120</v>
-      </c>
-      <c r="K68" t="s" s="3">
-        <v>121</v>
-      </c>
-      <c r="L68" t="s" s="3">
-        <v>122</v>
-      </c>
-      <c r="M68" t="s" s="3">
-        <v>123</v>
-      </c>
-      <c r="N68" t="s" s="3">
-        <v>124</v>
-      </c>
-      <c r="O68" t="s" s="3">
-        <v>125</v>
-      </c>
-      <c r="P68" t="s" s="3">
-        <v>126</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
       <c r="Q68" s="2"/>
       <c r="R68" s="2"/>
       <c r="S68" s="2"/>
@@ -8028,18 +7959,10 @@
       <c r="V68" s="2"/>
       <c r="W68" s="2"/>
       <c r="X68" s="2"/>
-      <c r="Y68" t="s" s="3">
-        <v>127</v>
-      </c>
-      <c r="Z68" t="s" s="3">
-        <v>128</v>
-      </c>
-      <c r="AA68" t="s" s="3">
-        <v>129</v>
-      </c>
-      <c r="AB68" t="s" s="3">
-        <v>130</v>
-      </c>
+      <c r="Y68" s="3"/>
+      <c r="Z68" s="3"/>
+      <c r="AA68" s="3"/>
+      <c r="AB68" s="3"/>
       <c r="AC68" s="2"/>
       <c r="AD68" s="12"/>
       <c r="AE68" s="12"/>

</xml_diff>

<commit_message>
fix: ecrf file fix
</commit_message>
<xml_diff>
--- a/app/templates/ecrf_template.xlsx
+++ b/app/templates/ecrf_template.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="217">
   <si>
     <t>Type</t>
   </si>
@@ -395,6 +395,12 @@
   </si>
   <si>
     <t>{{emission_n2o}}</t>
+  </si>
+  <si>
+    <t>{{emission_factor_description}}</t>
+  </si>
+  <si>
+    <t>{{emission_factor_source}}</t>
   </si>
   <si>
     <t>{{ghg_co2}}</t>
@@ -3100,20 +3106,24 @@
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
+      <c r="V2" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W2" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X2" s="2"/>
       <c r="Y2" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z2" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA2" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB2" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC2" s="2"/>
       <c r="AD2" s="12"/>
@@ -3126,7 +3136,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s" s="3">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s" s="3">
         <v>113</v>
@@ -3135,7 +3145,7 @@
         <v>114</v>
       </c>
       <c r="E3" t="s" s="3">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F3" t="s" s="3">
         <v>116</v>
@@ -3175,20 +3185,24 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
+      <c r="V3" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W3" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X3" s="2"/>
       <c r="Y3" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z3" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA3" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB3" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC3" s="2"/>
       <c r="AD3" s="12"/>
@@ -3201,7 +3215,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s" s="3">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s" s="3">
         <v>113</v>
@@ -3210,7 +3224,7 @@
         <v>114</v>
       </c>
       <c r="E4" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F4" t="s" s="3">
         <v>116</v>
@@ -3250,20 +3264,24 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
+      <c r="V4" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W4" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X4" s="2"/>
       <c r="Y4" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z4" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA4" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB4" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC4" s="2"/>
       <c r="AD4" s="12"/>
@@ -3276,13 +3294,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s" s="3">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D5" t="s" s="3">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E5" t="s" s="3">
         <v>115</v>
@@ -3325,20 +3343,24 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
+      <c r="V5" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W5" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X5" s="2"/>
       <c r="Y5" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z5" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA5" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB5" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC5" s="2"/>
       <c r="AD5" s="12"/>
@@ -3351,13 +3373,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s" s="3">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D6" t="s" s="3">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E6" t="s" s="3">
         <v>115</v>
@@ -3400,20 +3422,24 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
+      <c r="V6" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W6" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X6" s="2"/>
       <c r="Y6" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z6" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA6" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB6" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC6" s="2"/>
       <c r="AD6" s="12"/>
@@ -3426,16 +3452,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s" s="3">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C7" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D7" t="s" s="3">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E7" t="s" s="3">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F7" t="s" s="3">
         <v>116</v>
@@ -3475,20 +3501,24 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
+      <c r="V7" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W7" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X7" s="2"/>
       <c r="Y7" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z7" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA7" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB7" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC7" s="2"/>
       <c r="AD7" s="12"/>
@@ -3501,16 +3531,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C8" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D8" t="s" s="3">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E8" t="s" s="3">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F8" t="s" s="3">
         <v>116</v>
@@ -3550,20 +3580,24 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
+      <c r="V8" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W8" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X8" s="2"/>
       <c r="Y8" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z8" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA8" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB8" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC8" s="2"/>
       <c r="AD8" s="12"/>
@@ -3576,16 +3610,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s" s="3">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C9" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D9" t="s" s="3">
+        <v>138</v>
+      </c>
+      <c r="E9" t="s" s="3">
         <v>136</v>
-      </c>
-      <c r="E9" t="s" s="3">
-        <v>134</v>
       </c>
       <c r="F9" t="s" s="3">
         <v>116</v>
@@ -3625,20 +3659,24 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
+      <c r="V9" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W9" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X9" s="2"/>
       <c r="Y9" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z9" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA9" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB9" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC9" s="2"/>
       <c r="AD9" s="12"/>
@@ -3651,16 +3689,16 @@
         <v>1</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C10" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D10" t="s" s="3">
+        <v>138</v>
+      </c>
+      <c r="E10" t="s" s="3">
         <v>136</v>
-      </c>
-      <c r="E10" t="s" s="3">
-        <v>134</v>
       </c>
       <c r="F10" t="s" s="3">
         <v>116</v>
@@ -3700,20 +3738,24 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
+      <c r="V10" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W10" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X10" s="2"/>
       <c r="Y10" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z10" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA10" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB10" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC10" s="2"/>
       <c r="AD10" s="12"/>
@@ -3726,13 +3768,13 @@
         <v>1</v>
       </c>
       <c r="B11" t="s" s="3">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C11" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D11" t="s" s="3">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E11" t="s" s="3">
         <v>115</v>
@@ -3775,20 +3817,24 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
+      <c r="V11" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W11" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X11" s="2"/>
       <c r="Y11" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z11" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA11" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB11" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC11" s="2"/>
       <c r="AD11" s="12"/>
@@ -3801,16 +3847,16 @@
         <v>1</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C12" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D12" t="s" s="3">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E12" t="s" s="3">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F12" t="s" s="3">
         <v>116</v>
@@ -3850,20 +3896,24 @@
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
+      <c r="V12" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W12" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X12" s="2"/>
       <c r="Y12" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z12" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA12" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB12" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC12" s="2"/>
       <c r="AD12" s="12"/>
@@ -3876,16 +3926,16 @@
         <v>1</v>
       </c>
       <c r="B13" t="s" s="3">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C13" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D13" t="s" s="3">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E13" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F13" t="s" s="3">
         <v>116</v>
@@ -3925,20 +3975,24 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
+      <c r="V13" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W13" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X13" s="2"/>
       <c r="Y13" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z13" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA13" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB13" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC13" s="2"/>
       <c r="AD13" s="12"/>
@@ -3951,13 +4005,13 @@
         <v>1</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C14" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D14" t="s" s="3">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E14" t="s" s="3">
         <v>115</v>
@@ -4000,20 +4054,24 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
+      <c r="V14" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W14" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X14" s="2"/>
       <c r="Y14" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z14" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA14" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB14" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC14" s="2"/>
       <c r="AD14" s="12"/>
@@ -4026,13 +4084,13 @@
         <v>1</v>
       </c>
       <c r="B15" t="s" s="3">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C15" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D15" t="s" s="3">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E15" t="s" s="3">
         <v>115</v>
@@ -4075,20 +4133,24 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
+      <c r="V15" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W15" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X15" s="2"/>
       <c r="Y15" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z15" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA15" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB15" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC15" s="2"/>
       <c r="AD15" s="12"/>
@@ -4101,16 +4163,16 @@
         <v>1</v>
       </c>
       <c r="B16" t="s" s="3">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C16" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D16" t="s" s="3">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E16" t="s" s="3">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F16" t="s" s="3">
         <v>116</v>
@@ -4150,20 +4212,24 @@
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
+      <c r="V16" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W16" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X16" s="2"/>
       <c r="Y16" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z16" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA16" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB16" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC16" s="2"/>
       <c r="AD16" s="12"/>
@@ -4176,16 +4242,16 @@
         <v>1</v>
       </c>
       <c r="B17" t="s" s="3">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C17" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D17" t="s" s="3">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E17" t="s" s="3">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F17" t="s" s="3">
         <v>116</v>
@@ -4225,20 +4291,24 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
+      <c r="V17" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W17" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X17" s="2"/>
       <c r="Y17" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z17" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA17" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB17" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC17" s="2"/>
       <c r="AD17" s="12"/>
@@ -4251,16 +4321,16 @@
         <v>1</v>
       </c>
       <c r="B18" t="s" s="3">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C18" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D18" t="s" s="3">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E18" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F18" t="s" s="3">
         <v>116</v>
@@ -4300,20 +4370,24 @@
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
+      <c r="V18" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W18" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X18" s="2"/>
       <c r="Y18" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z18" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA18" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB18" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC18" s="2"/>
       <c r="AD18" s="12"/>
@@ -4326,16 +4400,16 @@
         <v>1</v>
       </c>
       <c r="B19" t="s" s="3">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C19" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D19" t="s" s="3">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E19" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F19" t="s" s="3">
         <v>116</v>
@@ -4375,20 +4449,24 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
+      <c r="V19" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W19" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X19" s="2"/>
       <c r="Y19" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z19" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA19" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB19" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC19" s="2"/>
       <c r="AD19" s="12"/>
@@ -4401,13 +4479,13 @@
         <v>1</v>
       </c>
       <c r="B20" t="s" s="3">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C20" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D20" t="s" s="3">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E20" t="s" s="3">
         <v>115</v>
@@ -4450,20 +4528,24 @@
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
+      <c r="V20" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W20" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X20" s="2"/>
       <c r="Y20" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z20" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA20" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB20" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC20" s="2"/>
       <c r="AD20" s="12"/>
@@ -4476,16 +4558,16 @@
         <v>1</v>
       </c>
       <c r="B21" t="s" s="3">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C21" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D21" t="s" s="3">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E21" t="s" s="3">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F21" t="s" s="3">
         <v>116</v>
@@ -4525,20 +4607,24 @@
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
+      <c r="V21" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W21" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X21" s="2"/>
       <c r="Y21" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z21" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA21" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB21" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC21" s="2"/>
       <c r="AD21" s="12"/>
@@ -4551,16 +4637,16 @@
         <v>1</v>
       </c>
       <c r="B22" t="s" s="3">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C22" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D22" t="s" s="3">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E22" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F22" t="s" s="3">
         <v>116</v>
@@ -4600,20 +4686,24 @@
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
+      <c r="V22" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W22" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X22" s="2"/>
       <c r="Y22" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z22" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA22" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB22" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC22" s="2"/>
       <c r="AD22" s="12"/>
@@ -4626,13 +4716,13 @@
         <v>1</v>
       </c>
       <c r="B23" t="s" s="3">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C23" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D23" t="s" s="3">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E23" t="s" s="3">
         <v>115</v>
@@ -4675,20 +4765,24 @@
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
+      <c r="V23" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W23" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X23" s="2"/>
       <c r="Y23" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z23" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA23" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB23" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC23" s="2"/>
       <c r="AD23" s="12"/>
@@ -4701,13 +4795,13 @@
         <v>1</v>
       </c>
       <c r="B24" t="s" s="3">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C24" t="s" s="3">
         <v>113</v>
       </c>
       <c r="D24" t="s" s="3">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E24" t="s" s="3">
         <v>115</v>
@@ -4750,20 +4844,24 @@
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
+      <c r="V24" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W24" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X24" s="2"/>
       <c r="Y24" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z24" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA24" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB24" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC24" s="2"/>
       <c r="AD24" s="12"/>
@@ -4780,10 +4878,10 @@
         <v>113</v>
       </c>
       <c r="D25" t="s" s="3">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E25" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F25" t="s" s="3">
         <v>116</v>
@@ -4823,20 +4921,24 @@
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
+      <c r="V25" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W25" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X25" s="2"/>
       <c r="Y25" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z25" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA25" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB25" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC25" s="2"/>
       <c r="AD25" s="12"/>
@@ -4849,13 +4951,13 @@
         <v>1</v>
       </c>
       <c r="B26" t="s" s="3">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C26" t="s" s="3">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D26" t="s" s="3">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E26" t="s" s="3">
         <v>115</v>
@@ -4898,20 +5000,24 @@
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
-      <c r="V26" s="2"/>
-      <c r="W26" s="2"/>
+      <c r="V26" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W26" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X26" s="2"/>
       <c r="Y26" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z26" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA26" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB26" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC26" s="2"/>
       <c r="AD26" s="12"/>
@@ -4924,16 +5030,16 @@
         <v>1</v>
       </c>
       <c r="B27" t="s" s="3">
+        <v>162</v>
+      </c>
+      <c r="C27" t="s" s="3">
         <v>160</v>
       </c>
-      <c r="C27" t="s" s="3">
-        <v>158</v>
-      </c>
       <c r="D27" t="s" s="3">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E27" t="s" s="3">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F27" t="s" s="3">
         <v>116</v>
@@ -4973,20 +5079,24 @@
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
-      <c r="W27" s="2"/>
+      <c r="V27" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W27" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X27" s="2"/>
       <c r="Y27" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z27" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA27" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB27" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC27" s="2"/>
       <c r="AD27" s="12"/>
@@ -4999,16 +5109,16 @@
         <v>1</v>
       </c>
       <c r="B28" t="s" s="3">
+        <v>163</v>
+      </c>
+      <c r="C28" t="s" s="3">
+        <v>160</v>
+      </c>
+      <c r="D28" t="s" s="3">
         <v>161</v>
       </c>
-      <c r="C28" t="s" s="3">
-        <v>158</v>
-      </c>
-      <c r="D28" t="s" s="3">
-        <v>159</v>
-      </c>
       <c r="E28" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F28" t="s" s="3">
         <v>116</v>
@@ -5048,20 +5158,24 @@
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
-      <c r="V28" s="2"/>
-      <c r="W28" s="2"/>
+      <c r="V28" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W28" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X28" s="2"/>
       <c r="Y28" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z28" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA28" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB28" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC28" s="2"/>
       <c r="AD28" s="12"/>
@@ -5074,13 +5188,13 @@
         <v>1</v>
       </c>
       <c r="B29" t="s" s="3">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C29" t="s" s="3">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D29" t="s" s="3">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E29" t="s" s="3">
         <v>115</v>
@@ -5123,20 +5237,24 @@
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
+      <c r="V29" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W29" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X29" s="2"/>
       <c r="Y29" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z29" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA29" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB29" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC29" s="2"/>
       <c r="AD29" s="12"/>
@@ -5149,16 +5267,16 @@
         <v>1</v>
       </c>
       <c r="B30" t="s" s="3">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C30" t="s" s="3">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D30" t="s" s="3">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E30" t="s" s="3">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F30" t="s" s="3">
         <v>116</v>
@@ -5198,20 +5316,24 @@
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
-      <c r="V30" s="2"/>
-      <c r="W30" s="2"/>
+      <c r="V30" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W30" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X30" s="2"/>
       <c r="Y30" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z30" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA30" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB30" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC30" s="2"/>
       <c r="AD30" s="12"/>
@@ -5224,16 +5346,16 @@
         <v>1</v>
       </c>
       <c r="B31" t="s" s="3">
+        <v>167</v>
+      </c>
+      <c r="C31" t="s" s="3">
+        <v>160</v>
+      </c>
+      <c r="D31" t="s" s="3">
         <v>165</v>
       </c>
-      <c r="C31" t="s" s="3">
-        <v>158</v>
-      </c>
-      <c r="D31" t="s" s="3">
-        <v>163</v>
-      </c>
       <c r="E31" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F31" t="s" s="3">
         <v>116</v>
@@ -5273,20 +5395,24 @@
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
-      <c r="W31" s="2"/>
+      <c r="V31" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W31" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X31" s="2"/>
       <c r="Y31" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z31" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA31" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB31" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC31" s="2"/>
       <c r="AD31" s="12"/>
@@ -5299,13 +5425,13 @@
         <v>1</v>
       </c>
       <c r="B32" t="s" s="3">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C32" t="s" s="3">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D32" t="s" s="3">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E32" t="s" s="3">
         <v>115</v>
@@ -5348,20 +5474,24 @@
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
-      <c r="V32" s="2"/>
-      <c r="W32" s="2"/>
+      <c r="V32" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W32" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X32" s="2"/>
       <c r="Y32" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z32" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA32" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB32" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC32" s="2"/>
       <c r="AD32" s="12"/>
@@ -5374,16 +5504,16 @@
         <v>1</v>
       </c>
       <c r="B33" t="s" s="3">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C33" t="s" s="3">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D33" t="s" s="3">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E33" t="s" s="3">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F33" t="s" s="3">
         <v>116</v>
@@ -5423,20 +5553,24 @@
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
-      <c r="V33" s="2"/>
-      <c r="W33" s="2"/>
+      <c r="V33" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W33" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X33" s="2"/>
       <c r="Y33" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z33" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA33" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB33" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC33" s="2"/>
       <c r="AD33" s="12"/>
@@ -5449,16 +5583,16 @@
         <v>1</v>
       </c>
       <c r="B34" t="s" s="3">
+        <v>171</v>
+      </c>
+      <c r="C34" t="s" s="3">
+        <v>160</v>
+      </c>
+      <c r="D34" t="s" s="3">
         <v>169</v>
       </c>
-      <c r="C34" t="s" s="3">
-        <v>158</v>
-      </c>
-      <c r="D34" t="s" s="3">
-        <v>167</v>
-      </c>
       <c r="E34" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F34" t="s" s="3">
         <v>116</v>
@@ -5498,20 +5632,24 @@
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
-      <c r="V34" s="2"/>
-      <c r="W34" s="2"/>
+      <c r="V34" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W34" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X34" s="2"/>
       <c r="Y34" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z34" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA34" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB34" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC34" s="2"/>
       <c r="AD34" s="12"/>
@@ -5524,13 +5662,13 @@
         <v>1</v>
       </c>
       <c r="B35" t="s" s="3">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C35" t="s" s="3">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D35" t="s" s="3">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E35" t="s" s="3">
         <v>115</v>
@@ -5573,20 +5711,24 @@
       <c r="S35" s="2"/>
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
-      <c r="V35" s="2"/>
-      <c r="W35" s="2"/>
+      <c r="V35" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W35" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X35" s="2"/>
       <c r="Y35" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z35" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA35" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB35" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC35" s="2"/>
       <c r="AD35" s="12"/>
@@ -5599,16 +5741,16 @@
         <v>1</v>
       </c>
       <c r="B36" t="s" s="3">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C36" t="s" s="3">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D36" t="s" s="3">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E36" t="s" s="3">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F36" t="s" s="3">
         <v>116</v>
@@ -5648,20 +5790,24 @@
       <c r="S36" s="2"/>
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
-      <c r="V36" s="2"/>
-      <c r="W36" s="2"/>
+      <c r="V36" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W36" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X36" s="2"/>
       <c r="Y36" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z36" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA36" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB36" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC36" s="2"/>
       <c r="AD36" s="12"/>
@@ -5674,16 +5820,16 @@
         <v>1</v>
       </c>
       <c r="B37" t="s" s="3">
+        <v>175</v>
+      </c>
+      <c r="C37" t="s" s="3">
+        <v>160</v>
+      </c>
+      <c r="D37" t="s" s="3">
         <v>173</v>
       </c>
-      <c r="C37" t="s" s="3">
-        <v>158</v>
-      </c>
-      <c r="D37" t="s" s="3">
-        <v>171</v>
-      </c>
       <c r="E37" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F37" t="s" s="3">
         <v>116</v>
@@ -5723,20 +5869,24 @@
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
-      <c r="V37" s="2"/>
-      <c r="W37" s="2"/>
+      <c r="V37" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W37" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X37" s="2"/>
       <c r="Y37" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z37" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA37" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB37" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="12"/>
@@ -5749,13 +5899,13 @@
         <v>1</v>
       </c>
       <c r="B38" t="s" s="3">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C38" t="s" s="3">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D38" t="s" s="3">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E38" t="s" s="3">
         <v>115</v>
@@ -5798,20 +5948,24 @@
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
-      <c r="V38" s="2"/>
-      <c r="W38" s="2"/>
+      <c r="V38" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W38" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X38" s="2"/>
       <c r="Y38" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z38" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA38" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB38" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC38" s="2"/>
       <c r="AD38" s="12"/>
@@ -5824,16 +5978,16 @@
         <v>1</v>
       </c>
       <c r="B39" t="s" s="3">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C39" t="s" s="3">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D39" t="s" s="3">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E39" t="s" s="3">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F39" t="s" s="3">
         <v>116</v>
@@ -5873,20 +6027,24 @@
       <c r="S39" s="2"/>
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
-      <c r="W39" s="2"/>
+      <c r="V39" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W39" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X39" s="2"/>
       <c r="Y39" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z39" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA39" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB39" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC39" s="2"/>
       <c r="AD39" s="12"/>
@@ -5899,16 +6057,16 @@
         <v>1</v>
       </c>
       <c r="B40" t="s" s="3">
+        <v>179</v>
+      </c>
+      <c r="C40" t="s" s="3">
+        <v>160</v>
+      </c>
+      <c r="D40" t="s" s="3">
         <v>177</v>
       </c>
-      <c r="C40" t="s" s="3">
-        <v>158</v>
-      </c>
-      <c r="D40" t="s" s="3">
-        <v>175</v>
-      </c>
       <c r="E40" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F40" t="s" s="3">
         <v>116</v>
@@ -5948,20 +6106,24 @@
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
-      <c r="V40" s="2"/>
-      <c r="W40" s="2"/>
+      <c r="V40" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W40" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X40" s="2"/>
       <c r="Y40" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z40" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA40" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB40" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC40" s="2"/>
       <c r="AD40" s="12"/>
@@ -5974,13 +6136,13 @@
         <v>1</v>
       </c>
       <c r="B41" t="s" s="3">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C41" t="s" s="3">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D41" t="s" s="3">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E41" t="s" s="3">
         <v>115</v>
@@ -6023,20 +6185,24 @@
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
-      <c r="V41" s="2"/>
-      <c r="W41" s="2"/>
+      <c r="V41" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W41" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X41" s="2"/>
       <c r="Y41" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z41" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA41" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB41" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC41" s="2"/>
       <c r="AD41" s="12"/>
@@ -6049,13 +6215,13 @@
         <v>1</v>
       </c>
       <c r="B42" t="s" s="3">
+        <v>183</v>
+      </c>
+      <c r="C42" t="s" s="3">
         <v>181</v>
       </c>
-      <c r="C42" t="s" s="3">
-        <v>179</v>
-      </c>
       <c r="D42" t="s" s="3">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E42" t="s" s="3">
         <v>115</v>
@@ -6098,20 +6264,24 @@
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
-      <c r="V42" s="2"/>
-      <c r="W42" s="2"/>
+      <c r="V42" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W42" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X42" s="2"/>
       <c r="Y42" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z42" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA42" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB42" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC42" s="2"/>
       <c r="AD42" s="12"/>
@@ -6124,16 +6294,16 @@
         <v>1</v>
       </c>
       <c r="B43" t="s" s="3">
+        <v>184</v>
+      </c>
+      <c r="C43" t="s" s="3">
+        <v>181</v>
+      </c>
+      <c r="D43" t="s" s="3">
         <v>182</v>
       </c>
-      <c r="C43" t="s" s="3">
-        <v>179</v>
-      </c>
-      <c r="D43" t="s" s="3">
-        <v>180</v>
-      </c>
       <c r="E43" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F43" t="s" s="3">
         <v>116</v>
@@ -6173,20 +6343,24 @@
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
-      <c r="V43" s="2"/>
-      <c r="W43" s="2"/>
+      <c r="V43" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W43" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X43" s="2"/>
       <c r="Y43" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z43" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA43" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB43" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC43" s="2"/>
       <c r="AD43" s="12"/>
@@ -6199,13 +6373,13 @@
         <v>1</v>
       </c>
       <c r="B44" t="s" s="3">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C44" t="s" s="3">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D44" t="s" s="3">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E44" t="s" s="3">
         <v>115</v>
@@ -6248,20 +6422,24 @@
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
-      <c r="V44" s="2"/>
-      <c r="W44" s="2"/>
+      <c r="V44" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W44" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X44" s="2"/>
       <c r="Y44" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z44" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA44" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB44" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC44" s="2"/>
       <c r="AD44" s="12"/>
@@ -6274,13 +6452,13 @@
         <v>1</v>
       </c>
       <c r="B45" t="s" s="3">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C45" t="s" s="3">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D45" t="s" s="3">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E45" t="s" s="3">
         <v>115</v>
@@ -6323,20 +6501,24 @@
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
-      <c r="V45" s="2"/>
-      <c r="W45" s="2"/>
+      <c r="V45" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W45" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X45" s="2"/>
       <c r="Y45" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z45" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA45" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB45" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC45" s="2"/>
       <c r="AD45" s="12"/>
@@ -6349,16 +6531,16 @@
         <v>1</v>
       </c>
       <c r="B46" t="s" s="3">
+        <v>188</v>
+      </c>
+      <c r="C46" t="s" s="3">
+        <v>181</v>
+      </c>
+      <c r="D46" t="s" s="3">
         <v>186</v>
       </c>
-      <c r="C46" t="s" s="3">
-        <v>179</v>
-      </c>
-      <c r="D46" t="s" s="3">
-        <v>184</v>
-      </c>
       <c r="E46" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F46" t="s" s="3">
         <v>116</v>
@@ -6398,20 +6580,24 @@
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
-      <c r="W46" s="2"/>
+      <c r="V46" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W46" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X46" s="2"/>
       <c r="Y46" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z46" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA46" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB46" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC46" s="2"/>
       <c r="AD46" s="12"/>
@@ -6424,13 +6610,13 @@
         <v>1</v>
       </c>
       <c r="B47" t="s" s="3">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C47" t="s" s="3">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D47" t="s" s="3">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E47" t="s" s="3">
         <v>115</v>
@@ -6473,20 +6659,24 @@
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
-      <c r="V47" s="2"/>
-      <c r="W47" s="2"/>
+      <c r="V47" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W47" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X47" s="2"/>
       <c r="Y47" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z47" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA47" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB47" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC47" s="2"/>
       <c r="AD47" s="12"/>
@@ -6499,13 +6689,13 @@
         <v>1</v>
       </c>
       <c r="B48" t="s" s="3">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C48" t="s" s="3">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D48" t="s" s="3">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E48" t="s" s="3">
         <v>115</v>
@@ -6548,20 +6738,24 @@
       <c r="S48" s="2"/>
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
-      <c r="V48" s="2"/>
-      <c r="W48" s="2"/>
+      <c r="V48" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W48" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X48" s="2"/>
       <c r="Y48" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z48" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA48" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB48" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC48" s="2"/>
       <c r="AD48" s="12"/>
@@ -6574,16 +6768,16 @@
         <v>1</v>
       </c>
       <c r="B49" t="s" s="3">
+        <v>192</v>
+      </c>
+      <c r="C49" t="s" s="3">
+        <v>181</v>
+      </c>
+      <c r="D49" t="s" s="3">
         <v>190</v>
       </c>
-      <c r="C49" t="s" s="3">
-        <v>179</v>
-      </c>
-      <c r="D49" t="s" s="3">
-        <v>188</v>
-      </c>
       <c r="E49" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F49" t="s" s="3">
         <v>116</v>
@@ -6623,20 +6817,24 @@
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
-      <c r="V49" s="2"/>
-      <c r="W49" s="2"/>
+      <c r="V49" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W49" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X49" s="2"/>
       <c r="Y49" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z49" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA49" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB49" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC49" s="2"/>
       <c r="AD49" s="12"/>
@@ -6649,13 +6847,13 @@
         <v>1</v>
       </c>
       <c r="B50" t="s" s="3">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C50" t="s" s="3">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D50" t="s" s="3">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E50" t="s" s="3">
         <v>115</v>
@@ -6698,20 +6896,24 @@
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
-      <c r="V50" s="2"/>
-      <c r="W50" s="2"/>
+      <c r="V50" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W50" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X50" s="2"/>
       <c r="Y50" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z50" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA50" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB50" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC50" s="2"/>
       <c r="AD50" s="12"/>
@@ -6724,13 +6926,13 @@
         <v>1</v>
       </c>
       <c r="B51" t="s" s="3">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C51" t="s" s="3">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D51" t="s" s="3">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E51" t="s" s="3">
         <v>115</v>
@@ -6773,20 +6975,24 @@
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
-      <c r="V51" s="2"/>
-      <c r="W51" s="2"/>
+      <c r="V51" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W51" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X51" s="2"/>
       <c r="Y51" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z51" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA51" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB51" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC51" s="2"/>
       <c r="AD51" s="12"/>
@@ -6799,16 +7005,16 @@
         <v>1</v>
       </c>
       <c r="B52" t="s" s="3">
+        <v>196</v>
+      </c>
+      <c r="C52" t="s" s="3">
+        <v>181</v>
+      </c>
+      <c r="D52" t="s" s="3">
         <v>194</v>
       </c>
-      <c r="C52" t="s" s="3">
-        <v>179</v>
-      </c>
-      <c r="D52" t="s" s="3">
-        <v>192</v>
-      </c>
       <c r="E52" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F52" t="s" s="3">
         <v>116</v>
@@ -6848,20 +7054,24 @@
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
-      <c r="V52" s="2"/>
-      <c r="W52" s="2"/>
+      <c r="V52" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W52" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X52" s="2"/>
       <c r="Y52" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z52" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA52" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB52" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC52" s="2"/>
       <c r="AD52" s="12"/>
@@ -6874,13 +7084,13 @@
         <v>1</v>
       </c>
       <c r="B53" t="s" s="3">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C53" t="s" s="3">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D53" t="s" s="3">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E53" t="s" s="3">
         <v>115</v>
@@ -6923,20 +7133,24 @@
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
-      <c r="V53" s="2"/>
-      <c r="W53" s="2"/>
+      <c r="V53" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W53" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X53" s="2"/>
       <c r="Y53" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z53" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA53" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB53" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC53" s="2"/>
       <c r="AD53" s="12"/>
@@ -6950,13 +7164,13 @@
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="3">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D54" t="s" s="3">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E54" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F54" t="s" s="3">
         <v>116</v>
@@ -6996,20 +7210,24 @@
       <c r="S54" s="2"/>
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
-      <c r="V54" s="2"/>
-      <c r="W54" s="2"/>
+      <c r="V54" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W54" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X54" s="2"/>
       <c r="Y54" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z54" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA54" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB54" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC54" s="2"/>
       <c r="AD54" s="12"/>
@@ -7022,13 +7240,13 @@
         <v>1</v>
       </c>
       <c r="B55" t="s" s="3">
+        <v>200</v>
+      </c>
+      <c r="C55" t="s" s="3">
         <v>198</v>
       </c>
-      <c r="C55" t="s" s="3">
-        <v>196</v>
-      </c>
       <c r="D55" t="s" s="3">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E55" t="s" s="3">
         <v>115</v>
@@ -7071,20 +7289,24 @@
       <c r="S55" s="2"/>
       <c r="T55" s="2"/>
       <c r="U55" s="2"/>
-      <c r="V55" s="2"/>
-      <c r="W55" s="2"/>
+      <c r="V55" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W55" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X55" s="2"/>
       <c r="Y55" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z55" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA55" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB55" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC55" s="2"/>
       <c r="AD55" s="12"/>
@@ -7098,13 +7320,13 @@
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="3">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D56" t="s" s="3">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E56" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F56" t="s" s="3">
         <v>116</v>
@@ -7144,20 +7366,24 @@
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
-      <c r="V56" s="2"/>
-      <c r="W56" s="2"/>
+      <c r="V56" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W56" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X56" s="2"/>
       <c r="Y56" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z56" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA56" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB56" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC56" s="2"/>
       <c r="AD56" s="12"/>
@@ -7170,13 +7396,13 @@
         <v>1</v>
       </c>
       <c r="B57" t="s" s="3">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C57" t="s" s="3">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D57" t="s" s="3">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E57" t="s" s="3">
         <v>115</v>
@@ -7219,20 +7445,24 @@
       <c r="S57" s="2"/>
       <c r="T57" s="2"/>
       <c r="U57" s="2"/>
-      <c r="V57" s="2"/>
-      <c r="W57" s="2"/>
+      <c r="V57" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W57" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X57" s="2"/>
       <c r="Y57" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z57" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA57" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB57" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC57" s="2"/>
       <c r="AD57" s="12"/>
@@ -7246,13 +7476,13 @@
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="3">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D58" t="s" s="3">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E58" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F58" t="s" s="3">
         <v>116</v>
@@ -7292,20 +7522,24 @@
       <c r="S58" s="2"/>
       <c r="T58" s="2"/>
       <c r="U58" s="2"/>
-      <c r="V58" s="2"/>
-      <c r="W58" s="2"/>
+      <c r="V58" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W58" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X58" s="2"/>
       <c r="Y58" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z58" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA58" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB58" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC58" s="2"/>
       <c r="AD58" s="12"/>
@@ -7318,13 +7552,13 @@
         <v>1</v>
       </c>
       <c r="B59" t="s" s="3">
+        <v>205</v>
+      </c>
+      <c r="C59" t="s" s="3">
         <v>203</v>
       </c>
-      <c r="C59" t="s" s="3">
-        <v>201</v>
-      </c>
       <c r="D59" t="s" s="3">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E59" t="s" s="3">
         <v>115</v>
@@ -7367,20 +7601,24 @@
       <c r="S59" s="2"/>
       <c r="T59" s="2"/>
       <c r="U59" s="2"/>
-      <c r="V59" s="2"/>
-      <c r="W59" s="2"/>
+      <c r="V59" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W59" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X59" s="2"/>
       <c r="Y59" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z59" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA59" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB59" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC59" s="2"/>
       <c r="AD59" s="12"/>
@@ -7394,13 +7632,13 @@
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="3">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D60" t="s" s="3">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E60" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F60" t="s" s="3">
         <v>116</v>
@@ -7440,20 +7678,24 @@
       <c r="S60" s="2"/>
       <c r="T60" s="2"/>
       <c r="U60" s="2"/>
-      <c r="V60" s="2"/>
-      <c r="W60" s="2"/>
+      <c r="V60" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W60" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X60" s="2"/>
       <c r="Y60" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z60" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA60" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB60" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC60" s="2"/>
       <c r="AD60" s="12"/>
@@ -7466,13 +7708,13 @@
         <v>1</v>
       </c>
       <c r="B61" t="s" s="3">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C61" t="s" s="3">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D61" t="s" s="3">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E61" t="s" s="3">
         <v>115</v>
@@ -7515,20 +7757,24 @@
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
       <c r="U61" s="2"/>
-      <c r="V61" s="2"/>
-      <c r="W61" s="2"/>
+      <c r="V61" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W61" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X61" s="2"/>
       <c r="Y61" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z61" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA61" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB61" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC61" s="2"/>
       <c r="AD61" s="12"/>
@@ -7542,13 +7788,13 @@
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="3">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D62" t="s" s="3">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E62" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F62" t="s" s="3">
         <v>116</v>
@@ -7588,20 +7834,24 @@
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
       <c r="U62" s="2"/>
-      <c r="V62" s="2"/>
-      <c r="W62" s="2"/>
+      <c r="V62" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W62" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X62" s="2"/>
       <c r="Y62" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z62" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA62" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB62" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC62" s="2"/>
       <c r="AD62" s="12"/>
@@ -7614,13 +7864,13 @@
         <v>1</v>
       </c>
       <c r="B63" t="s" s="3">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C63" t="s" s="3">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D63" t="s" s="3">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E63" t="s" s="3">
         <v>115</v>
@@ -7663,20 +7913,24 @@
       <c r="S63" s="2"/>
       <c r="T63" s="2"/>
       <c r="U63" s="2"/>
-      <c r="V63" s="2"/>
-      <c r="W63" s="2"/>
+      <c r="V63" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W63" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X63" s="2"/>
       <c r="Y63" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z63" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA63" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB63" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC63" s="2"/>
       <c r="AD63" s="12"/>
@@ -7689,13 +7943,13 @@
         <v>1</v>
       </c>
       <c r="B64" t="s" s="3">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C64" t="s" s="3">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D64" t="s" s="3">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E64" t="s" s="3">
         <v>115</v>
@@ -7738,20 +7992,24 @@
       <c r="S64" s="2"/>
       <c r="T64" s="2"/>
       <c r="U64" s="2"/>
-      <c r="V64" s="2"/>
-      <c r="W64" s="2"/>
+      <c r="V64" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W64" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X64" s="2"/>
       <c r="Y64" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z64" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA64" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB64" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC64" s="2"/>
       <c r="AD64" s="12"/>
@@ -7764,13 +8022,13 @@
         <v>1</v>
       </c>
       <c r="B65" t="s" s="3">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C65" t="s" s="3">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D65" t="s" s="3">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E65" t="s" s="3">
         <v>115</v>
@@ -7813,20 +8071,24 @@
       <c r="S65" s="2"/>
       <c r="T65" s="2"/>
       <c r="U65" s="2"/>
-      <c r="V65" s="2"/>
-      <c r="W65" s="2"/>
+      <c r="V65" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="W65" t="s" s="3">
+        <v>128</v>
+      </c>
       <c r="X65" s="2"/>
       <c r="Y65" t="s" s="3">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z65" t="s" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AA65" t="s" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AB65" t="s" s="3">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AC65" s="2"/>
       <c r="AD65" s="12"/>
@@ -7840,13 +8102,13 @@
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="3">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D66" t="s" s="3">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E66" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F66" s="3"/>
       <c r="G66" t="s" s="3">
@@ -7885,13 +8147,13 @@
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="3">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D67" t="s" s="3">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E67" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" t="s" s="3">
@@ -7930,13 +8192,13 @@
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="3">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D68" t="s" s="3">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E68" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F68" s="3"/>
       <c r="G68" t="s" s="3">
@@ -7975,13 +8237,13 @@
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="3">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D69" t="s" s="3">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E69" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" t="s" s="3">
@@ -8020,10 +8282,10 @@
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="3">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D70" t="s" s="3">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E70" t="s" s="3">
         <v>115</v>
@@ -8064,16 +8326,16 @@
         <v>1</v>
       </c>
       <c r="B71" t="s" s="3">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C71" t="s" s="3">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D71" t="s" s="3">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E71" t="s" s="3">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F71" s="3"/>
       <c r="G71" t="s" s="3">

</xml_diff>